<commit_message>
Add Github Actions CI/CD
</commit_message>
<xml_diff>
--- a/cervical_predictions_final.xlsx
+++ b/cervical_predictions_final.xlsx
@@ -712,13 +712,13 @@
         <v>0</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.1723968237638474</v>
+        <v>0.158631294965744</v>
       </c>
       <c r="AG2" t="n">
         <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.1744918462634087</v>
+        <v>0.174315647482872</v>
       </c>
     </row>
     <row r="3">
@@ -828,13 +828,13 @@
         <v>1</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.7321831583976746</v>
+        <v>0.7352001070976257</v>
       </c>
       <c r="AG3" t="n">
         <v>1</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.7629102337360383</v>
+        <v>0.7601000535488129</v>
       </c>
     </row>
     <row r="4">
@@ -944,13 +944,13 @@
         <v>0</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.2399623095989227</v>
+        <v>0.2161490470170975</v>
       </c>
       <c r="AG4" t="n">
         <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.2589030688802401</v>
+        <v>0.2477411901752154</v>
       </c>
     </row>
     <row r="5">
@@ -1060,13 +1060,13 @@
         <v>1</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.8267048597335815</v>
+        <v>0.8370144963264465</v>
       </c>
       <c r="AG5" t="n">
         <v>1</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.8032719902197518</v>
+        <v>0.8207989148298898</v>
       </c>
     </row>
     <row r="6">
@@ -1176,13 +1176,13 @@
         <v>1</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.8688667416572571</v>
+        <v>0.8211670517921448</v>
       </c>
       <c r="AG6" t="n">
         <v>1</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.7912787001875294</v>
+        <v>0.7629539471414937</v>
       </c>
     </row>
     <row r="7">
@@ -1292,13 +1292,13 @@
         <v>0</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.1358885914087296</v>
+        <v>0.1323568969964981</v>
       </c>
       <c r="AG7" t="n">
         <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.1782569148299872</v>
+        <v>0.1803668521998106</v>
       </c>
     </row>
     <row r="8">
@@ -1408,13 +1408,13 @@
         <v>1</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.9788889288902283</v>
+        <v>0.9728147387504578</v>
       </c>
       <c r="AG8" t="n">
         <v>1</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.9292762923240662</v>
+        <v>0.9289073693752289</v>
       </c>
     </row>
     <row r="9">
@@ -1524,13 +1524,13 @@
         <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.3112846612930298</v>
+        <v>0.265093207359314</v>
       </c>
       <c r="AG9" t="n">
         <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.2975925061967638</v>
+        <v>0.2746160481241015</v>
       </c>
     </row>
     <row r="10">
@@ -1640,13 +1640,13 @@
         <v>1</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.9845393300056458</v>
+        <v>0.9780120849609375</v>
       </c>
       <c r="AG10" t="n">
         <v>1</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.9731029999256133</v>
+        <v>0.9715060424804687</v>
       </c>
     </row>
     <row r="11">
@@ -1756,13 +1756,13 @@
         <v>0</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.130503311753273</v>
+        <v>0.1396342813968658</v>
       </c>
       <c r="AG11" t="n">
         <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.1354663425087929</v>
+        <v>0.1425671406984329</v>
       </c>
     </row>
     <row r="12">
@@ -1872,13 +1872,13 @@
         <v>0</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.2179665714502335</v>
+        <v>0.2170718014240265</v>
       </c>
       <c r="AG12" t="n">
         <v>0</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.2195506573589707</v>
+        <v>0.2262064472707177</v>
       </c>
     </row>
     <row r="13">
@@ -1988,13 +1988,13 @@
         <v>0</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.1968400925397873</v>
+        <v>0.2321974635124207</v>
       </c>
       <c r="AG13" t="n">
         <v>0</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.1689853120446205</v>
+        <v>0.1750674817562103</v>
       </c>
     </row>
     <row r="14">
@@ -2104,13 +2104,13 @@
         <v>1</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.8857305645942688</v>
+        <v>0.8915439248085022</v>
       </c>
       <c r="AG14" t="n">
         <v>1</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.8726419270038605</v>
+        <v>0.8582719624042511</v>
       </c>
     </row>
     <row r="15">
@@ -2220,13 +2220,13 @@
         <v>1</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.9495120048522949</v>
+        <v>0.935580849647522</v>
       </c>
       <c r="AG15" t="n">
         <v>1</v>
       </c>
       <c r="AH15" t="n">
-        <v>0.897103218793869</v>
+        <v>0.891290424823761</v>
       </c>
     </row>
     <row r="16">
@@ -2336,13 +2336,13 @@
         <v>0</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.02704577147960663</v>
+        <v>0.0231169443577528</v>
       </c>
       <c r="AG16" t="n">
         <v>0</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.114161884256753</v>
+        <v>0.1182931213016834</v>
       </c>
     </row>
     <row r="17">
@@ -2452,13 +2452,13 @@
         <v>0</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.102064274251461</v>
+        <v>0.1196410730481148</v>
       </c>
       <c r="AG17" t="n">
         <v>0</v>
       </c>
       <c r="AH17" t="n">
-        <v>0.1012210382024447</v>
+        <v>0.1127372031907241</v>
       </c>
     </row>
     <row r="18">
@@ -2568,13 +2568,13 @@
         <v>0</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.2143108546733856</v>
+        <v>0.2109549045562744</v>
       </c>
       <c r="AG18" t="n">
         <v>0</v>
       </c>
       <c r="AH18" t="n">
-        <v>0.2458141461309036</v>
+        <v>0.2415632918771347</v>
       </c>
     </row>
     <row r="19">
@@ -2684,13 +2684,13 @@
         <v>0</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.02255231887102127</v>
+        <v>0.02037015184760094</v>
       </c>
       <c r="AG19" t="n">
         <v>0</v>
       </c>
       <c r="AH19" t="n">
-        <v>0.05515909099578858</v>
+        <v>0.05293507592380047</v>
       </c>
     </row>
     <row r="20">
@@ -2800,13 +2800,13 @@
         <v>0</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.173184409737587</v>
+        <v>0.1770026832818985</v>
       </c>
       <c r="AG20" t="n">
         <v>0</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.1914928968956596</v>
+        <v>0.1877776574304229</v>
       </c>
     </row>
     <row r="21">
@@ -2916,13 +2916,13 @@
         <v>1</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.820350170135498</v>
+        <v>0.8293185234069824</v>
       </c>
       <c r="AG21" t="n">
         <v>1</v>
       </c>
       <c r="AH21" t="n">
-        <v>0.7621277207742658</v>
+        <v>0.7692376608262983</v>
       </c>
     </row>
     <row r="22">
@@ -3032,13 +3032,13 @@
         <v>0</v>
       </c>
       <c r="AF22" t="n">
-        <v>0.0725623294711113</v>
+        <v>0.0731637179851532</v>
       </c>
       <c r="AG22" t="n">
         <v>0</v>
       </c>
       <c r="AH22" t="n">
-        <v>0.1279925010115431</v>
+        <v>0.126774841448717</v>
       </c>
     </row>
     <row r="23">
@@ -3148,13 +3148,13 @@
         <v>0</v>
       </c>
       <c r="AF23" t="n">
-        <v>0.4620386958122253</v>
+        <v>0.4870985746383667</v>
       </c>
       <c r="AG23" t="n">
         <v>0</v>
       </c>
       <c r="AH23" t="n">
-        <v>0.4785024575885376</v>
+        <v>0.4835101269181808</v>
       </c>
     </row>
     <row r="24">
@@ -3264,13 +3264,13 @@
         <v>0</v>
       </c>
       <c r="AF24" t="n">
-        <v>0.08076939731836319</v>
+        <v>0.07497644424438477</v>
       </c>
       <c r="AG24" t="n">
         <v>0</v>
       </c>
       <c r="AH24" t="n">
-        <v>0.1125360699207114</v>
+        <v>0.1021812045783327</v>
       </c>
     </row>
     <row r="25">
@@ -3380,13 +3380,13 @@
         <v>1</v>
       </c>
       <c r="AF25" t="n">
-        <v>0.8771073222160339</v>
+        <v>0.8920946717262268</v>
       </c>
       <c r="AG25" t="n">
         <v>1</v>
       </c>
       <c r="AH25" t="n">
-        <v>0.8151005579895444</v>
+        <v>0.8297834469742246</v>
       </c>
     </row>
     <row r="26">
@@ -3496,13 +3496,13 @@
         <v>1</v>
       </c>
       <c r="AF26" t="n">
-        <v>0.9593200087547302</v>
+        <v>0.9386615753173828</v>
       </c>
       <c r="AG26" t="n">
         <v>1</v>
       </c>
       <c r="AH26" t="n">
-        <v>0.9248481762409211</v>
+        <v>0.9143307876586915</v>
       </c>
     </row>
     <row r="27">
@@ -3612,13 +3612,13 @@
         <v>1</v>
       </c>
       <c r="AF27" t="n">
-        <v>0.9547404050827026</v>
+        <v>0.9487159252166748</v>
       </c>
       <c r="AG27" t="n">
         <v>1</v>
       </c>
       <c r="AH27" t="n">
-        <v>0.9535400950908661</v>
+        <v>0.9518579626083374</v>
       </c>
     </row>
     <row r="28">
@@ -3728,13 +3728,13 @@
         <v>0</v>
       </c>
       <c r="AF28" t="n">
-        <v>0.02134492807090282</v>
+        <v>0.0307955015450716</v>
       </c>
       <c r="AG28" t="n">
         <v>0</v>
       </c>
       <c r="AH28" t="n">
-        <v>0.05090800492713848</v>
+        <v>0.05550191743920246</v>
       </c>
     </row>
     <row r="29">
@@ -3844,13 +3844,13 @@
         <v>0</v>
       </c>
       <c r="AF29" t="n">
-        <v>0.2729825973510742</v>
+        <v>0.3521316051483154</v>
       </c>
       <c r="AG29" t="n">
         <v>0</v>
       </c>
       <c r="AH29" t="n">
-        <v>0.3145421583149476</v>
+        <v>0.3338225025627656</v>
       </c>
     </row>
     <row r="30">
@@ -3960,13 +3960,13 @@
         <v>0</v>
       </c>
       <c r="AF30" t="n">
-        <v>0.1439969539642334</v>
+        <v>0.111082062125206</v>
       </c>
       <c r="AG30" t="n">
         <v>0</v>
       </c>
       <c r="AH30" t="n">
-        <v>0.1335982569750389</v>
+        <v>0.1206268706616005</v>
       </c>
     </row>
     <row r="31">
@@ -4077,13 +4077,13 @@
         <v>1</v>
       </c>
       <c r="AF31" t="n">
-        <v>0.7811641097068787</v>
+        <v>0.79853755235672</v>
       </c>
       <c r="AG31" t="n">
         <v>1</v>
       </c>
       <c r="AH31" t="n">
-        <v>0.7302184257117836</v>
+        <v>0.733090952357444</v>
       </c>
     </row>
     <row r="32">
@@ -4193,13 +4193,13 @@
         <v>0</v>
       </c>
       <c r="AF32" t="n">
-        <v>0.4620386958122253</v>
+        <v>0.4870985746383667</v>
       </c>
       <c r="AG32" t="n">
         <v>0</v>
       </c>
       <c r="AH32" t="n">
-        <v>0.4785024575885376</v>
+        <v>0.4835101269181808</v>
       </c>
     </row>
     <row r="33">
@@ -4309,13 +4309,13 @@
         <v>0</v>
       </c>
       <c r="AF33" t="n">
-        <v>0.05003475770354271</v>
+        <v>0.05767790600657463</v>
       </c>
       <c r="AG33" t="n">
         <v>0</v>
       </c>
       <c r="AH33" t="n">
-        <v>0.08085826989616218</v>
+        <v>0.087302768792761</v>
       </c>
     </row>
     <row r="34">
@@ -4425,13 +4425,13 @@
         <v>1</v>
       </c>
       <c r="AF34" t="n">
-        <v>0.8334425687789917</v>
+        <v>0.796573281288147</v>
       </c>
       <c r="AG34" t="n">
         <v>1</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.7606927544515227</v>
+        <v>0.7490804285447692</v>
       </c>
     </row>
     <row r="35">
@@ -4541,13 +4541,13 @@
         <v>1</v>
       </c>
       <c r="AF35" t="n">
-        <v>0.9827054738998413</v>
+        <v>0.9808639287948608</v>
       </c>
       <c r="AG35" t="n">
         <v>1</v>
       </c>
       <c r="AH35" t="n">
-        <v>0.959497629404068</v>
+        <v>0.9579319643974304</v>
       </c>
     </row>
     <row r="36">
@@ -4657,13 +4657,13 @@
         <v>1</v>
       </c>
       <c r="AF36" t="n">
-        <v>0.9831444025039673</v>
+        <v>0.9799086451530457</v>
       </c>
       <c r="AG36" t="n">
         <v>1</v>
       </c>
       <c r="AH36" t="n">
-        <v>0.9717950320243836</v>
+        <v>0.9687043225765228</v>
       </c>
     </row>
     <row r="37">
@@ -4773,13 +4773,13 @@
         <v>1</v>
       </c>
       <c r="AF37" t="n">
-        <v>0.8568621873855591</v>
+        <v>0.8334342837333679</v>
       </c>
       <c r="AG37" t="n">
         <v>1</v>
       </c>
       <c r="AH37" t="n">
-        <v>0.7627626942124575</v>
+        <v>0.7430496202435701</v>
       </c>
     </row>
     <row r="38">
@@ -4889,13 +4889,13 @@
         <v>1</v>
       </c>
       <c r="AF38" t="n">
-        <v>0.9880802035331726</v>
+        <v>0.9856091141700745</v>
       </c>
       <c r="AG38" t="n">
         <v>1</v>
       </c>
       <c r="AH38" t="n">
-        <v>0.9827462017536164</v>
+        <v>0.9803045570850373</v>
       </c>
     </row>
     <row r="39">
@@ -5005,13 +5005,13 @@
         <v>0</v>
       </c>
       <c r="AF39" t="n">
-        <v>0.1758978664875031</v>
+        <v>0.1691986918449402</v>
       </c>
       <c r="AG39" t="n">
         <v>0</v>
       </c>
       <c r="AH39" t="n">
-        <v>0.1935771223513215</v>
+        <v>0.1888277721015542</v>
       </c>
     </row>
     <row r="40">
@@ -5121,13 +5121,13 @@
         <v>1</v>
       </c>
       <c r="AF40" t="n">
-        <v>0.9925292134284973</v>
+        <v>0.9895609617233276</v>
       </c>
       <c r="AG40" t="n">
         <v>1</v>
       </c>
       <c r="AH40" t="n">
-        <v>0.9733724677562714</v>
+        <v>0.9722804808616639</v>
       </c>
     </row>
     <row r="41">
@@ -5237,13 +5237,13 @@
         <v>1</v>
       </c>
       <c r="AF41" t="n">
-        <v>0.8102267980575562</v>
+        <v>0.847390353679657</v>
       </c>
       <c r="AG41" t="n">
         <v>1</v>
       </c>
       <c r="AH41" t="n">
-        <v>0.7771940767716157</v>
+        <v>0.7964637815903413</v>
       </c>
     </row>
     <row r="42">
@@ -5353,13 +5353,13 @@
         <v>1</v>
       </c>
       <c r="AF42" t="n">
-        <v>0.735005259513855</v>
+        <v>0.7388190031051636</v>
       </c>
       <c r="AG42" t="n">
         <v>1</v>
       </c>
       <c r="AH42" t="n">
-        <v>0.7820256160895029</v>
+        <v>0.7618261682192484</v>
       </c>
     </row>
     <row r="43">
@@ -5469,13 +5469,13 @@
         <v>0</v>
       </c>
       <c r="AF43" t="n">
-        <v>0.03881528601050377</v>
+        <v>0.02961660362780094</v>
       </c>
       <c r="AG43" t="n">
         <v>0</v>
       </c>
       <c r="AH43" t="n">
-        <v>0.03644801035876337</v>
+        <v>0.03608461760337416</v>
       </c>
     </row>
     <row r="44">
@@ -5585,13 +5585,13 @@
         <v>0</v>
       </c>
       <c r="AF44" t="n">
-        <v>0.006200028583407402</v>
+        <v>0.007333073299378157</v>
       </c>
       <c r="AG44" t="n">
         <v>0</v>
       </c>
       <c r="AH44" t="n">
-        <v>0.03994607318383031</v>
+        <v>0.04069682069313102</v>
       </c>
     </row>
     <row r="45">
@@ -5701,13 +5701,13 @@
         <v>0</v>
       </c>
       <c r="AF45" t="n">
-        <v>0.06355796754360199</v>
+        <v>0.06650502234697342</v>
       </c>
       <c r="AG45" t="n">
         <v>0</v>
       </c>
       <c r="AH45" t="n">
-        <v>0.1143479124270784</v>
+        <v>0.1110327952169286</v>
       </c>
     </row>
     <row r="46">
@@ -5818,13 +5818,13 @@
         <v>1</v>
       </c>
       <c r="AF46" t="n">
-        <v>0.7086272835731506</v>
+        <v>0.7735996246337891</v>
       </c>
       <c r="AG46" t="n">
         <v>1</v>
       </c>
       <c r="AH46" t="n">
-        <v>0.6742830074098376</v>
+        <v>0.7072442567613391</v>
       </c>
     </row>
     <row r="47">
@@ -5934,13 +5934,13 @@
         <v>0</v>
       </c>
       <c r="AF47" t="n">
-        <v>0.04042802751064301</v>
+        <v>0.05580199882388115</v>
       </c>
       <c r="AG47" t="n">
         <v>0</v>
       </c>
       <c r="AH47" t="n">
-        <v>0.09326799560360044</v>
+        <v>0.0978717596458587</v>
       </c>
     </row>
     <row r="48">
@@ -6050,13 +6050,13 @@
         <v>0</v>
       </c>
       <c r="AF48" t="n">
-        <v>0.004896584898233414</v>
+        <v>0.005403688177466393</v>
       </c>
       <c r="AG48" t="n">
         <v>0</v>
       </c>
       <c r="AH48" t="n">
-        <v>0.03551788449539813</v>
+        <v>0.0348987947988418</v>
       </c>
     </row>
     <row r="49">
@@ -6166,13 +6166,13 @@
         <v>1</v>
       </c>
       <c r="AF49" t="n">
-        <v>0.9678245782852173</v>
+        <v>0.9276770949363708</v>
       </c>
       <c r="AG49" t="n">
         <v>1</v>
       </c>
       <c r="AH49" t="n">
-        <v>0.9090551960468292</v>
+        <v>0.8938385474681854</v>
       </c>
     </row>
     <row r="50">
@@ -6282,13 +6282,13 @@
         <v>1</v>
       </c>
       <c r="AF50" t="n">
-        <v>0.9811180233955383</v>
+        <v>0.9763912558555603</v>
       </c>
       <c r="AG50" t="n">
         <v>1</v>
       </c>
       <c r="AH50" t="n">
-        <v>0.9666695877710978</v>
+        <v>0.9647372945944468</v>
       </c>
     </row>
     <row r="51">
@@ -6398,13 +6398,13 @@
         <v>0</v>
       </c>
       <c r="AF51" t="n">
-        <v>0.03233255818486214</v>
+        <v>0.02816156111657619</v>
       </c>
       <c r="AG51" t="n">
         <v>0</v>
       </c>
       <c r="AH51" t="n">
-        <v>0.09811955014864604</v>
+        <v>0.09293494722495477</v>
       </c>
     </row>
     <row r="52">
@@ -6514,13 +6514,13 @@
         <v>1</v>
       </c>
       <c r="AF52" t="n">
-        <v>0.5161174535751343</v>
+        <v>0.5080369710922241</v>
       </c>
       <c r="AG52" t="n">
         <v>1</v>
       </c>
       <c r="AH52" t="n">
-        <v>0.5436687253581154</v>
+        <v>0.5542962633238899</v>
       </c>
     </row>
     <row r="53">
@@ -6630,13 +6630,13 @@
         <v>0</v>
       </c>
       <c r="AF53" t="n">
-        <v>0.1640803515911102</v>
+        <v>0.1860285997390747</v>
       </c>
       <c r="AG53" t="n">
         <v>0</v>
       </c>
       <c r="AH53" t="n">
-        <v>0.2142337398678845</v>
+        <v>0.2128662379533833</v>
       </c>
     </row>
     <row r="54">
@@ -6746,13 +6746,13 @@
         <v>0</v>
       </c>
       <c r="AF54" t="n">
-        <v>0.09279733151197433</v>
+        <v>0.08220406621694565</v>
       </c>
       <c r="AG54" t="n">
         <v>0</v>
       </c>
       <c r="AH54" t="n">
-        <v>0.1839231725825511</v>
+        <v>0.1746503997637474</v>
       </c>
     </row>
     <row r="55">
@@ -6862,13 +6862,13 @@
         <v>1</v>
       </c>
       <c r="AF55" t="n">
-        <v>0.7314448952674866</v>
+        <v>0.6995736956596375</v>
       </c>
       <c r="AG55" t="n">
         <v>1</v>
       </c>
       <c r="AH55" t="n">
-        <v>0.7793666156875345</v>
+        <v>0.7793656024085733</v>
       </c>
     </row>
     <row r="56">
@@ -6978,13 +6978,13 @@
         <v>1</v>
       </c>
       <c r="AF56" t="n">
-        <v>0.9799110889434814</v>
+        <v>0.9815338253974915</v>
       </c>
       <c r="AG56" t="n">
         <v>1</v>
       </c>
       <c r="AH56" t="n">
-        <v>0.9642763922214508</v>
+        <v>0.9667669126987457</v>
       </c>
     </row>
     <row r="57">
@@ -7094,13 +7094,13 @@
         <v>0</v>
       </c>
       <c r="AF57" t="n">
-        <v>0.1474915593862534</v>
+        <v>0.1775864958763123</v>
       </c>
       <c r="AG57" t="n">
         <v>0</v>
       </c>
       <c r="AH57" t="n">
-        <v>0.1639804546332598</v>
+        <v>0.1846707542038203</v>
       </c>
     </row>
     <row r="58">
@@ -7210,13 +7210,13 @@
         <v>0</v>
       </c>
       <c r="AF58" t="n">
-        <v>0.01166301034390926</v>
+        <v>0.01534297876060009</v>
       </c>
       <c r="AG58" t="n">
         <v>0</v>
       </c>
       <c r="AH58" t="n">
-        <v>0.05262739358469844</v>
+        <v>0.05267148938030004</v>
       </c>
     </row>
     <row r="59">
@@ -7326,13 +7326,13 @@
         <v>0</v>
       </c>
       <c r="AF59" t="n">
-        <v>0.0707133412361145</v>
+        <v>0.07328317314386368</v>
       </c>
       <c r="AG59" t="n">
         <v>0</v>
       </c>
       <c r="AH59" t="n">
-        <v>0.1214379207292829</v>
+        <v>0.120651392737988</v>
       </c>
     </row>
     <row r="60">
@@ -7442,13 +7442,13 @@
         <v>0</v>
       </c>
       <c r="AF60" t="n">
-        <v>0.1166622564196587</v>
+        <v>0.1405758261680603</v>
       </c>
       <c r="AG60" t="n">
         <v>0</v>
       </c>
       <c r="AH60" t="n">
-        <v>0.2018724389274915</v>
+        <v>0.2124649964173635</v>
       </c>
     </row>
     <row r="61">
@@ -7558,13 +7558,13 @@
         <v>1</v>
       </c>
       <c r="AF61" t="n">
-        <v>0.9635182619094849</v>
+        <v>0.9549438953399658</v>
       </c>
       <c r="AG61" t="n">
         <v>1</v>
       </c>
       <c r="AH61" t="n">
-        <v>0.9405914469559988</v>
+        <v>0.9383052810033163</v>
       </c>
     </row>
     <row r="62">
@@ -7674,13 +7674,13 @@
         <v>0</v>
       </c>
       <c r="AF62" t="n">
-        <v>0.1078498363494873</v>
+        <v>0.09061343222856522</v>
       </c>
       <c r="AG62" t="n">
         <v>0</v>
       </c>
       <c r="AH62" t="n">
-        <v>0.1165446364834089</v>
+        <v>0.1215513707651873</v>
       </c>
     </row>
     <row r="63">
@@ -7790,13 +7790,13 @@
         <v>0</v>
       </c>
       <c r="AF63" t="n">
-        <v>0.07597765326499939</v>
+        <v>0.07439254224300385</v>
       </c>
       <c r="AG63" t="n">
         <v>0</v>
       </c>
       <c r="AH63" t="n">
-        <v>0.08373872942252765</v>
+        <v>0.08015857270880351</v>
       </c>
     </row>
     <row r="64">
@@ -7906,13 +7906,13 @@
         <v>1</v>
       </c>
       <c r="AF64" t="n">
-        <v>0.9657663702964783</v>
+        <v>0.9558704495429993</v>
       </c>
       <c r="AG64" t="n">
         <v>1</v>
       </c>
       <c r="AH64" t="n">
-        <v>0.8873322454149073</v>
+        <v>0.8830971565896815</v>
       </c>
     </row>
     <row r="65">
@@ -8022,13 +8022,13 @@
         <v>0</v>
       </c>
       <c r="AF65" t="n">
-        <v>0.1026327610015869</v>
+        <v>0.1116232201457024</v>
       </c>
       <c r="AG65" t="n">
         <v>0</v>
       </c>
       <c r="AH65" t="n">
-        <v>0.1552800417145093</v>
+        <v>0.1628636934061845</v>
       </c>
     </row>
     <row r="66">
@@ -8139,13 +8139,13 @@
         <v>1</v>
       </c>
       <c r="AF66" t="n">
-        <v>0.780964195728302</v>
+        <v>0.8201408982276917</v>
       </c>
       <c r="AG66" t="n">
         <v>1</v>
       </c>
       <c r="AH66" t="n">
-        <v>0.8025156688690185</v>
+        <v>0.7988204491138458</v>
       </c>
     </row>
     <row r="67">
@@ -8255,13 +8255,13 @@
         <v>1</v>
       </c>
       <c r="AF67" t="n">
-        <v>0.9966744184494019</v>
+        <v>0.9965772032737732</v>
       </c>
       <c r="AG67" t="n">
         <v>1</v>
       </c>
       <c r="AH67" t="n">
-        <v>0.9806142282485961</v>
+        <v>0.9807886016368865</v>
       </c>
     </row>
     <row r="68">
@@ -8371,13 +8371,13 @@
         <v>1</v>
       </c>
       <c r="AF68" t="n">
-        <v>0.9603393077850342</v>
+        <v>0.9680298566818237</v>
       </c>
       <c r="AG68" t="n">
         <v>1</v>
       </c>
       <c r="AH68" t="n">
-        <v>0.9452181527614594</v>
+        <v>0.9475149283409119</v>
       </c>
     </row>
     <row r="69">
@@ -8487,13 +8487,13 @@
         <v>0</v>
       </c>
       <c r="AF69" t="n">
-        <v>0.04452505707740784</v>
+        <v>0.04266458004713058</v>
       </c>
       <c r="AG69" t="n">
         <v>0</v>
       </c>
       <c r="AH69" t="n">
-        <v>0.05875961599250634</v>
+        <v>0.05966562335689862</v>
       </c>
     </row>
     <row r="70">
@@ -8603,13 +8603,13 @@
         <v>1</v>
       </c>
       <c r="AF70" t="n">
-        <v>0.8541721105575562</v>
+        <v>0.8549113273620605</v>
       </c>
       <c r="AG70" t="n">
         <v>1</v>
       </c>
       <c r="AH70" t="n">
-        <v>0.7276890111718753</v>
+        <v>0.7275336516652683</v>
       </c>
     </row>
     <row r="71">
@@ -8719,13 +8719,13 @@
         <v>0</v>
       </c>
       <c r="AF71" t="n">
-        <v>0.02353697083890438</v>
+        <v>0.01550623122602701</v>
       </c>
       <c r="AG71" t="n">
         <v>0</v>
       </c>
       <c r="AH71" t="n">
-        <v>0.03451197081059218</v>
+        <v>0.02912811561301351</v>
       </c>
     </row>
     <row r="72">
@@ -8836,13 +8836,13 @@
         <v>1</v>
       </c>
       <c r="AF72" t="n">
-        <v>0.9011656641960144</v>
+        <v>0.9415588974952698</v>
       </c>
       <c r="AG72" t="n">
         <v>1</v>
       </c>
       <c r="AH72" t="n">
-        <v>0.8812882220745086</v>
+        <v>0.8995294487476349</v>
       </c>
     </row>
     <row r="73">
@@ -8952,13 +8952,13 @@
         <v>1</v>
       </c>
       <c r="AF73" t="n">
-        <v>0.8568993210792542</v>
+        <v>0.8422042727470398</v>
       </c>
       <c r="AG73" t="n">
         <v>1</v>
       </c>
       <c r="AH73" t="n">
-        <v>0.8714112710952759</v>
+        <v>0.86610213637352</v>
       </c>
     </row>
     <row r="74">
@@ -9068,13 +9068,13 @@
         <v>0</v>
       </c>
       <c r="AF74" t="n">
-        <v>0.07267015427350998</v>
+        <v>0.05519074201583862</v>
       </c>
       <c r="AG74" t="n">
         <v>0</v>
       </c>
       <c r="AH74" t="n">
-        <v>0.0813767091350423</v>
+        <v>0.07912314878569709</v>
       </c>
     </row>
     <row r="75">
@@ -9184,13 +9184,13 @@
         <v>1</v>
       </c>
       <c r="AF75" t="n">
-        <v>0.9144737124443054</v>
+        <v>0.9088230133056641</v>
       </c>
       <c r="AG75" t="n">
         <v>1</v>
       </c>
       <c r="AH75" t="n">
-        <v>0.9132636304696401</v>
+        <v>0.9196198399861654</v>
       </c>
     </row>
     <row r="76">
@@ -9300,13 +9300,13 @@
         <v>1</v>
       </c>
       <c r="AF76" t="n">
-        <v>0.9939889907836914</v>
+        <v>0.9936195015907288</v>
       </c>
       <c r="AG76" t="n">
         <v>1</v>
       </c>
       <c r="AH76" t="n">
-        <v>0.9929284719626108</v>
+        <v>0.993476417462031</v>
       </c>
     </row>
     <row r="77">
@@ -9420,13 +9420,13 @@
         <v>0</v>
       </c>
       <c r="AF77" t="n">
-        <v>0.1326271593570709</v>
+        <v>0.129927784204483</v>
       </c>
       <c r="AG77" t="n">
         <v>0</v>
       </c>
       <c r="AH77" t="n">
-        <v>0.1219801870981852</v>
+        <v>0.1241305587689082</v>
       </c>
     </row>
     <row r="78">
@@ -9536,13 +9536,13 @@
         <v>0</v>
       </c>
       <c r="AF78" t="n">
-        <v>0.02018621563911438</v>
+        <v>0.02239401824772358</v>
       </c>
       <c r="AG78" t="n">
         <v>0</v>
       </c>
       <c r="AH78" t="n">
-        <v>0.03144327502697707</v>
+        <v>0.03119700912386179</v>
       </c>
     </row>
     <row r="79">
@@ -9652,13 +9652,13 @@
         <v>0</v>
       </c>
       <c r="AF79" t="n">
-        <v>0.05593280494213104</v>
+        <v>0.09506458044052124</v>
       </c>
       <c r="AG79" t="n">
         <v>0</v>
       </c>
       <c r="AH79" t="n">
-        <v>0.1189488253200447</v>
+        <v>0.1342791995609199</v>
       </c>
     </row>
     <row r="80">
@@ -9769,13 +9769,13 @@
         <v>1</v>
       </c>
       <c r="AF80" t="n">
-        <v>0.8685616254806519</v>
+        <v>0.8504944443702698</v>
       </c>
       <c r="AG80" t="n">
         <v>1</v>
       </c>
       <c r="AH80" t="n">
-        <v>0.8209867427265728</v>
+        <v>0.8152408847725475</v>
       </c>
     </row>
     <row r="81">
@@ -9885,13 +9885,13 @@
         <v>1</v>
       </c>
       <c r="AF81" t="n">
-        <v>0.5772968530654907</v>
+        <v>0.5633867383003235</v>
       </c>
       <c r="AG81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH81" t="n">
-        <v>0.4977648072779436</v>
+        <v>0.5181648247778674</v>
       </c>
     </row>
     <row r="82">
@@ -10001,13 +10001,13 @@
         <v>0</v>
       </c>
       <c r="AF82" t="n">
-        <v>0.499710738658905</v>
+        <v>0.489534467458725</v>
       </c>
       <c r="AG82" t="n">
         <v>1</v>
       </c>
       <c r="AH82" t="n">
-        <v>0.5894597079753876</v>
+        <v>0.5873609837293625</v>
       </c>
     </row>
     <row r="83">
@@ -10117,13 +10117,13 @@
         <v>1</v>
       </c>
       <c r="AF83" t="n">
-        <v>0.9344746470451355</v>
+        <v>0.94016033411026</v>
       </c>
       <c r="AG83" t="n">
         <v>1</v>
       </c>
       <c r="AH83" t="n">
-        <v>0.9347183048725128</v>
+        <v>0.93258016705513</v>
       </c>
     </row>
     <row r="84">
@@ -10233,13 +10233,13 @@
         <v>0</v>
       </c>
       <c r="AF84" t="n">
-        <v>0.009702829644083977</v>
+        <v>0.00871607568114996</v>
       </c>
       <c r="AG84" t="n">
         <v>0</v>
       </c>
       <c r="AH84" t="n">
-        <v>0.06575458531205852</v>
+        <v>0.06653512117390831</v>
       </c>
     </row>
     <row r="85">
@@ -10349,13 +10349,13 @@
         <v>0</v>
       </c>
       <c r="AF85" t="n">
-        <v>0.1010568216443062</v>
+        <v>0.09498370438814163</v>
       </c>
       <c r="AG85" t="n">
         <v>0</v>
       </c>
       <c r="AH85" t="n">
-        <v>0.1420259654337452</v>
+        <v>0.144682328384547</v>
       </c>
     </row>
     <row r="86">
@@ -10465,13 +10465,13 @@
         <v>0</v>
       </c>
       <c r="AF86" t="n">
-        <v>0.136813759803772</v>
+        <v>0.1290431469678879</v>
       </c>
       <c r="AG86" t="n">
         <v>0</v>
       </c>
       <c r="AH86" t="n">
-        <v>0.2100662401782142</v>
+        <v>0.2052993512617217</v>
       </c>
     </row>
     <row r="87">
@@ -10582,13 +10582,13 @@
         <v>1</v>
       </c>
       <c r="AF87" t="n">
-        <v>0.97381591796875</v>
+        <v>0.9708641767501831</v>
       </c>
       <c r="AG87" t="n">
         <v>1</v>
       </c>
       <c r="AH87" t="n">
-        <v>0.8563176817099254</v>
+        <v>0.8548487550417583</v>
       </c>
     </row>
     <row r="88">
@@ -10698,13 +10698,13 @@
         <v>1</v>
       </c>
       <c r="AF88" t="n">
-        <v>0.9586769938468933</v>
+        <v>0.9753211140632629</v>
       </c>
       <c r="AG88" t="n">
         <v>1</v>
       </c>
       <c r="AH88" t="n">
-        <v>0.9501540625095368</v>
+        <v>0.9526605570316315</v>
       </c>
     </row>
     <row r="89">
@@ -10814,13 +10814,13 @@
         <v>0</v>
       </c>
       <c r="AF89" t="n">
-        <v>0.4468786716461182</v>
+        <v>0.4452976584434509</v>
       </c>
       <c r="AG89" t="n">
         <v>0</v>
       </c>
       <c r="AH89" t="n">
-        <v>0.409403331319491</v>
+        <v>0.3833154958883921</v>
       </c>
     </row>
     <row r="90">
@@ -10930,13 +10930,13 @@
         <v>1</v>
       </c>
       <c r="AF90" t="n">
-        <v>0.9537578225135803</v>
+        <v>0.9626352787017822</v>
       </c>
       <c r="AG90" t="n">
         <v>1</v>
       </c>
       <c r="AH90" t="n">
-        <v>0.9466141956647238</v>
+        <v>0.9581509726842246</v>
       </c>
     </row>
     <row r="91">
@@ -11046,13 +11046,13 @@
         <v>1</v>
       </c>
       <c r="AF91" t="n">
-        <v>0.7362935543060303</v>
+        <v>0.7904155254364014</v>
       </c>
       <c r="AG91" t="n">
         <v>1</v>
       </c>
       <c r="AH91" t="n">
-        <v>0.7344310936133067</v>
+        <v>0.7503431793848674</v>
       </c>
     </row>
     <row r="92">
@@ -11162,13 +11162,13 @@
         <v>0</v>
       </c>
       <c r="AF92" t="n">
-        <v>0.1469345837831497</v>
+        <v>0.1402952820062637</v>
       </c>
       <c r="AG92" t="n">
         <v>0</v>
       </c>
       <c r="AH92" t="n">
-        <v>0.1739879098534584</v>
+        <v>0.1713976410031319</v>
       </c>
     </row>
     <row r="93">
@@ -11278,13 +11278,13 @@
         <v>1</v>
       </c>
       <c r="AF93" t="n">
-        <v>0.835204541683197</v>
+        <v>0.7978374361991882</v>
       </c>
       <c r="AG93" t="n">
         <v>1</v>
       </c>
       <c r="AH93" t="n">
-        <v>0.7911585407968446</v>
+        <v>0.77724571402034</v>
       </c>
     </row>
     <row r="94">
@@ -11394,13 +11394,13 @@
         <v>0</v>
       </c>
       <c r="AF94" t="n">
-        <v>0.04277489334344864</v>
+        <v>0.0404176339507103</v>
       </c>
       <c r="AG94" t="n">
         <v>0</v>
       </c>
       <c r="AH94" t="n">
-        <v>0.1039510809282462</v>
+        <v>0.1022817336420218</v>
       </c>
     </row>
     <row r="95">
@@ -11510,13 +11510,13 @@
         <v>0</v>
       </c>
       <c r="AF95" t="n">
-        <v>0.499710738658905</v>
+        <v>0.489534467458725</v>
       </c>
       <c r="AG95" t="n">
         <v>0</v>
       </c>
       <c r="AH95" t="n">
-        <v>0.4094597079753876</v>
+        <v>0.4073609837293625</v>
       </c>
     </row>
     <row r="96">
@@ -11626,13 +11626,13 @@
         <v>0</v>
       </c>
       <c r="AF96" t="n">
-        <v>0.1466121077537537</v>
+        <v>0.1519044935703278</v>
       </c>
       <c r="AG96" t="n">
         <v>0</v>
       </c>
       <c r="AH96" t="n">
-        <v>0.1377198537356324</v>
+        <v>0.159563357896275</v>
       </c>
     </row>
     <row r="97">
@@ -11742,13 +11742,13 @@
         <v>1</v>
       </c>
       <c r="AF97" t="n">
-        <v>0.9181660413742065</v>
+        <v>0.9215932488441467</v>
       </c>
       <c r="AG97" t="n">
         <v>1</v>
       </c>
       <c r="AH97" t="n">
-        <v>0.9281809043884277</v>
+        <v>0.9307966244220733</v>
       </c>
     </row>
     <row r="98">
@@ -11858,13 +11858,13 @@
         <v>0</v>
       </c>
       <c r="AF98" t="n">
-        <v>0.01166301034390926</v>
+        <v>0.01534297876060009</v>
       </c>
       <c r="AG98" t="n">
         <v>0</v>
       </c>
       <c r="AH98" t="n">
-        <v>0.05262739358469844</v>
+        <v>0.05267148938030004</v>
       </c>
     </row>
     <row r="99">
@@ -11974,13 +11974,13 @@
         <v>0</v>
       </c>
       <c r="AF99" t="n">
-        <v>0.05980763211846352</v>
+        <v>0.06647927314043045</v>
       </c>
       <c r="AG99" t="n">
         <v>0</v>
       </c>
       <c r="AH99" t="n">
-        <v>0.1017439825998412</v>
+        <v>0.09976741434799301</v>
       </c>
     </row>
     <row r="100">
@@ -12090,13 +12090,13 @@
         <v>1</v>
       </c>
       <c r="AF100" t="n">
-        <v>0.9713370800018311</v>
+        <v>0.9606019258499146</v>
       </c>
       <c r="AG100" t="n">
         <v>1</v>
       </c>
       <c r="AH100" t="n">
-        <v>0.9488657975196839</v>
+        <v>0.9453009629249574</v>
       </c>
     </row>
     <row r="101">
@@ -12206,13 +12206,13 @@
         <v>1</v>
       </c>
       <c r="AF101" t="n">
-        <v>0.9790785312652588</v>
+        <v>0.9700343608856201</v>
       </c>
       <c r="AG101" t="n">
         <v>1</v>
       </c>
       <c r="AH101" t="n">
-        <v>0.979066481590271</v>
+        <v>0.97501718044281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>